<commit_message>
fix steel LCI input for blast furnace slag. Change to "market for blast furnace slag" to avoid issue with inexistent dataset in EN15804.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-steel.xlsx
+++ b/premise/data/additional_inventories/lci-steel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54256BC1-04B2-444C-9014-76AF3325992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBB2BFD-47BF-8243-963E-C3654FBEA17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5630,7 +5630,7 @@
   <dimension ref="A1:R157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5905,7 +5905,7 @@
         <v>489</v>
       </c>
       <c r="B13" s="29">
-        <v>0</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>270</v>
@@ -10236,7 +10236,7 @@
   <dimension ref="A1:R139"/>
   <sheetViews>
     <sheetView zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10511,7 +10511,7 @@
         <v>489</v>
       </c>
       <c r="B13" s="29">
-        <v>0</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>270</v>
@@ -14446,7 +14446,7 @@
   <dimension ref="A1:R156"/>
   <sheetViews>
     <sheetView zoomScale="111" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14721,7 +14721,7 @@
         <v>489</v>
       </c>
       <c r="B13" s="29">
-        <v>0</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>270</v>

</xml_diff>